<commit_message>
New Commit on 08/17
</commit_message>
<xml_diff>
--- a/Test Case/eApp Test Data.xlsx
+++ b/Test Case/eApp Test Data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eAppAutomation\Test Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D387725D-EAF8-454D-938B-FC41B95FB8EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="10_ncr:100000_{D387725D-EAF8-454D-938B-FC41B95FB8EB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="4160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="2" windowHeight="4160" windowWidth="16200" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCase" sheetId="1" r:id="rId1"/>
-    <sheet name="TestData" sheetId="2" r:id="rId2"/>
-    <sheet name="TestData (2)" sheetId="4" r:id="rId3"/>
-    <sheet name="ListValues" sheetId="3" r:id="rId4"/>
+    <sheet name="TestCase" r:id="rId1" sheetId="1"/>
+    <sheet name="TestData" r:id="rId2" sheetId="2"/>
+    <sheet name="TestData (2)" r:id="rId3" sheetId="4"/>
+    <sheet name="ListValues" r:id="rId4" sheetId="3"/>
   </sheets>
   <definedNames>
     <definedName name="P_Country">ListValues!$D$2:$D$24</definedName>
@@ -31,7 +31,7 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="172">
   <si>
     <t>SLNo</t>
   </si>
@@ -541,12 +541,28 @@
   </si>
   <si>
     <t>08/05/2018</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>$60,000</t>
+  </si>
+  <si>
+    <t>1988-12-08</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>1995-01-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -667,82 +683,98 @@
     </border>
   </borders>
   <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="49">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="4">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal_OLI_LU_NATION" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal_OLI_LUEXT_SUFFIX" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal_Sheet2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal_Sheet4" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -759,10 +791,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -797,7 +829,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -849,7 +881,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -960,21 +992,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -991,7 +1023,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1043,16 +1075,16 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -1060,8 +1092,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1099,19 +1131,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="list" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>P_Yes_No</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1119,9 +1151,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.81640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1135,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row ht="43.5" r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
@@ -1370,49 +1402,49 @@
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:C7" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B7:C7" type="list" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>P_Suffix</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:C8" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B8:C8" type="list" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>P_States</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:C9 B14:C15 B18:C18 B20:C24" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B9:C9 B14:C15 B18:C18 B20:C24" type="list" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>P_Yes_No</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:C13" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B13:C13" type="list" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>P_Gender</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:C16" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B16:C16" type="list" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>P_UWClass</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:C17" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B17:C17" type="list" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>P_Frequency</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:C3" xr:uid="{00000000-0002-0000-0100-000006000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B3:C3" type="list" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>P_PlanofInsurance</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52F2985-23B5-4103-BDA8-163FD22005C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52F2985-23B5-4103-BDA8-163FD22005C0}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <selection activeCell="E7" pane="bottomLeft" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="38.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1663,9 +1695,11 @@
       <c r="C16" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="25" t="s">
-        <v>165</v>
+      <c r="D16" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1889,8 +1923,12 @@
       <c r="C30" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="26"/>
+      <c r="D30" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
@@ -1902,8 +1940,12 @@
       <c r="C31" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="27"/>
+      <c r="D31" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
@@ -1915,8 +1957,12 @@
       <c r="C32" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="28"/>
+      <c r="D32" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
@@ -1928,8 +1974,12 @@
       <c r="C33" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="29"/>
+      <c r="D33" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
@@ -1941,8 +1991,12 @@
       <c r="C34" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="30"/>
+      <c r="D34" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="46" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
@@ -1954,8 +2008,12 @@
       <c r="C35" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="31"/>
+      <c r="D35" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="47" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
@@ -1967,38 +2025,42 @@
       <c r="C36" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D36" s="24"/>
-      <c r="E36" s="32"/>
+      <c r="D36" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21:E21" xr:uid="{63BF2A67-F2B3-4C32-A201-03503A960558}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D21:E21" type="list" xr:uid="{63BF2A67-F2B3-4C32-A201-03503A960558}">
       <formula1>P_Frequency</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20:E20" xr:uid="{94FFB3B2-D830-4E80-8C74-1F62E2705CEC}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D20:E20" type="list" xr:uid="{94FFB3B2-D830-4E80-8C74-1F62E2705CEC}">
       <formula1>P_UWClass</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:E17" xr:uid="{9E71B626-1F3E-4FB0-8918-E2EBF903A19C}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D17:E17" type="list" xr:uid="{9E71B626-1F3E-4FB0-8918-E2EBF903A19C}">
       <formula1>P_Gender</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:E28 D22:E22 D13:E13 D18:E18" xr:uid="{F815C3B6-49CC-4934-9685-0B640082F958}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D24:E28 D22:E22 D13:E13 D18:E18" type="list" xr:uid="{F815C3B6-49CC-4934-9685-0B640082F958}">
       <formula1>P_Yes_No</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:E12" xr:uid="{91BC0295-88CC-4EF7-AE5C-056C624E6EB5}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D12:E12" type="list" xr:uid="{91BC0295-88CC-4EF7-AE5C-056C624E6EB5}">
       <formula1>P_States</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{21814D12-6B4D-41CC-BDC0-E0E585335FE7}">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C3:C1048576" type="list" xr:uid="{21814D12-6B4D-41CC-BDC0-E0E585335FE7}">
       <formula1>Step</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
@@ -2006,11 +2068,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="23.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.54296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.54296875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.26953125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="19.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -2487,6 +2549,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Path changes for new laptop
</commit_message>
<xml_diff>
--- a/Test Case/eApp Test Data.xlsx
+++ b/Test Case/eApp Test Data.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="193">
   <si>
     <t>SLNo</t>
   </si>
@@ -752,7 +752,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="55">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -820,6 +820,14 @@
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1860,7 +1868,7 @@
       <c r="C16" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="47" t="s">
         <v>191</v>
       </c>
       <c r="E16" s="17"/>
@@ -2162,7 +2170,7 @@
       <c r="C30" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="48" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="18" t="s">
@@ -2185,7 +2193,7 @@
       <c r="C31" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="49" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="19" t="s">
@@ -2208,7 +2216,7 @@
       <c r="C32" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="50" t="s">
         <v>166</v>
       </c>
       <c r="E32" s="20" t="s">
@@ -2231,7 +2239,7 @@
       <c r="C33" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="51" t="s">
         <v>167</v>
       </c>
       <c r="E33" s="21" t="s">
@@ -2254,7 +2262,7 @@
       <c r="C34" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D34" s="44" t="s">
+      <c r="D34" s="52" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="22" t="s">
@@ -2277,7 +2285,7 @@
       <c r="C35" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D35" s="45" t="s">
+      <c r="D35" s="53" t="s">
         <v>47</v>
       </c>
       <c r="E35" s="23" t="s">
@@ -2300,7 +2308,7 @@
       <c r="C36" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D36" s="46" t="s">
+      <c r="D36" s="54" t="s">
         <v>47</v>
       </c>
       <c r="E36" s="24" t="s">

</xml_diff>